<commit_message>
Update after testing API
</commit_message>
<xml_diff>
--- a/Document/Testing/Testing API in Postman.xlsx
+++ b/Document/Testing/Testing API in Postman.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\happyfarmprg4\Document\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F81D0AB-0F5A-45DD-8DDD-3B55DCF77D56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C071789C-1660-41D2-AB1C-37D6CF6B7EDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{932464D8-E0C0-4E04-A057-D57ACE00B7DA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="28">
   <si>
     <t>Role</t>
   </si>
@@ -72,16 +72,10 @@
     <t>Region</t>
   </si>
   <si>
-    <t>Keluar pesan Berhasil menambah region tapi ga kesimpen di db</t>
-  </si>
-  <si>
     <t>Testing API in Postman</t>
   </si>
   <si>
     <t>Category</t>
-  </si>
-  <si>
-    <t>Keluar pesan Berhasil menambah tapi ga kesimpen di db</t>
   </si>
   <si>
     <t>SubDistrict</t>
@@ -94,9 +88,6 @@
 </t>
   </si>
   <si>
-    <t>Keluar pesan Berhasil mengubah tapi ga keubah di db</t>
-  </si>
-  <si>
     <t>Goods</t>
   </si>
   <si>
@@ -110,6 +101,15 @@
   </si>
   <si>
     <t>Error : System.Data.Entity.Validation.DbEntityValidationException: 'Validation failed for one or more entities. See 'EntityValidationErrors' property for more details.'</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>Admin Produksi</t>
+  </si>
+  <si>
+    <t>Error : The ObjectContext instance has been disposed and can no longer be used for operations that require a connection.</t>
   </si>
 </sst>
 </file>
@@ -471,22 +471,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10E974AC-ED86-4ABA-98C6-9F30F49BB8C4}">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40:C44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70:D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -557,7 +557,7 @@
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -594,13 +594,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
@@ -608,7 +608,7 @@
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
@@ -637,7 +637,7 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
@@ -680,13 +680,13 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C28" t="s">
         <v>6</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
@@ -694,7 +694,7 @@
         <v>9</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
@@ -702,7 +702,7 @@
         <v>8</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
@@ -710,7 +710,7 @@
         <v>11</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
@@ -718,81 +718,290 @@
         <v>12</v>
       </c>
       <c r="D32" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>23</v>
+      </c>
+      <c r="C40" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>23</v>
-      </c>
-      <c r="C34" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
-        <v>9</v>
-      </c>
-      <c r="D35" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
-        <v>8</v>
-      </c>
-      <c r="D36" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
-        <v>11</v>
-      </c>
-      <c r="D37" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
-        <v>12</v>
-      </c>
-      <c r="D38" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
+      <c r="B46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>9</v>
+      </c>
+      <c r="D47" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>12</v>
+      </c>
+      <c r="D50" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>14</v>
+      </c>
+      <c r="C52" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>8</v>
+      </c>
+      <c r="D54" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>11</v>
+      </c>
+      <c r="D55" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>12</v>
+      </c>
+      <c r="D56" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>17</v>
+      </c>
+      <c r="C58" t="s">
+        <v>6</v>
+      </c>
+      <c r="D58" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>9</v>
+      </c>
+      <c r="D59" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>8</v>
+      </c>
+      <c r="D60" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>11</v>
+      </c>
+      <c r="D61" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>12</v>
+      </c>
+      <c r="D62" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>26</v>
       </c>
-      <c r="C40" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" t="s">
+      <c r="B64" t="s">
+        <v>20</v>
+      </c>
+      <c r="C64" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
+        <v>12</v>
+      </c>
+      <c r="D68" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C42" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C44" t="s">
-        <v>12</v>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>16</v>
+      </c>
+      <c r="C70" t="s">
+        <v>6</v>
+      </c>
+      <c r="D70" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>9</v>
+      </c>
+      <c r="D71" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
+        <v>8</v>
+      </c>
+      <c r="D72" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C73" t="s">
+        <v>11</v>
+      </c>
+      <c r="D73" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
+        <v>12</v>
+      </c>
+      <c r="D74" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>